<commit_message>
added universities dataset and its description
</commit_message>
<xml_diff>
--- a/data_information.xlsx
+++ b/data_information.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="180">
   <si>
     <t xml:space="preserve">Filename</t>
   </si>
@@ -563,6 +563,24 @@
   <si>
     <t xml:space="preserve">Total sunshine duration</t>
   </si>
+  <si>
+    <t xml:space="preserve">THE_UK_Universities_ranking.ods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top universities in the UK 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.timeshighereducation.com/student/best-universities/best-universities-uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK Rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution</t>
+  </si>
 </sst>
 </file>
 
@@ -575,7 +593,7 @@
     <numFmt numFmtId="167" formatCode="0%"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -641,6 +659,12 @@
       <name val="Consolas"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1025,7 +1049,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1328,6 +1352,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1409,10 +1437,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M264"/>
+  <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A242" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G260" activeCellId="0" sqref="G260"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A257" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F275" activeCellId="0" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5923,6 +5951,51 @@
       <c r="L247" s="30"/>
       <c r="M247" s="30"/>
     </row>
+    <row r="248" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0"/>
+      <c r="B248" s="0"/>
+      <c r="C248" s="0"/>
+      <c r="D248" s="0"/>
+      <c r="E248" s="0"/>
+      <c r="F248" s="0"/>
+      <c r="G248" s="0"/>
+      <c r="H248" s="0"/>
+      <c r="I248" s="0"/>
+      <c r="J248" s="0"/>
+      <c r="K248" s="0"/>
+      <c r="L248" s="0"/>
+      <c r="M248" s="0"/>
+    </row>
+    <row r="249" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0"/>
+      <c r="B249" s="0"/>
+      <c r="C249" s="0"/>
+      <c r="D249" s="0"/>
+      <c r="E249" s="0"/>
+      <c r="F249" s="0"/>
+      <c r="G249" s="0"/>
+      <c r="H249" s="0"/>
+      <c r="I249" s="0"/>
+      <c r="J249" s="0"/>
+      <c r="K249" s="0"/>
+      <c r="L249" s="0"/>
+      <c r="M249" s="0"/>
+    </row>
+    <row r="250" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0"/>
+      <c r="B250" s="0"/>
+      <c r="C250" s="0"/>
+      <c r="D250" s="0"/>
+      <c r="E250" s="0"/>
+      <c r="F250" s="0"/>
+      <c r="G250" s="0"/>
+      <c r="H250" s="0"/>
+      <c r="I250" s="0"/>
+      <c r="J250" s="0"/>
+      <c r="K250" s="0"/>
+      <c r="L250" s="0"/>
+      <c r="M250" s="0"/>
+    </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
         <v>0</v>
@@ -6211,8 +6284,228 @@
       <c r="L264" s="2"/>
       <c r="M264" s="2"/>
     </row>
+    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C268" s="3"/>
+      <c r="D268" s="3"/>
+      <c r="E268" s="3"/>
+      <c r="F268" s="3"/>
+      <c r="G268" s="3"/>
+      <c r="H268" s="3"/>
+      <c r="I268" s="3"/>
+      <c r="J268" s="3"/>
+      <c r="K268" s="3"/>
+      <c r="L268" s="3"/>
+      <c r="M268" s="3"/>
+    </row>
+    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C269" s="3"/>
+      <c r="D269" s="3"/>
+      <c r="E269" s="3"/>
+      <c r="F269" s="3"/>
+      <c r="G269" s="3"/>
+      <c r="H269" s="3"/>
+      <c r="I269" s="3"/>
+      <c r="J269" s="3"/>
+      <c r="K269" s="3"/>
+      <c r="L269" s="3"/>
+      <c r="M269" s="3"/>
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B270" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="C270" s="3"/>
+      <c r="D270" s="3"/>
+      <c r="E270" s="3"/>
+      <c r="F270" s="3"/>
+      <c r="G270" s="3"/>
+      <c r="H270" s="3"/>
+      <c r="I270" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J270" s="3" t="n">
+        <v>2018</v>
+      </c>
+      <c r="K270" s="3"/>
+      <c r="L270" s="3"/>
+      <c r="M270" s="3"/>
+    </row>
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B271" s="2"/>
+      <c r="C271" s="6" t="n">
+        <v>90</v>
+      </c>
+      <c r="D271" s="6"/>
+      <c r="E271" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F271" s="4"/>
+      <c r="G271" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H271" s="6"/>
+      <c r="I271" s="6"/>
+      <c r="J271" s="6"/>
+      <c r="K271" s="6"/>
+      <c r="L271" s="6"/>
+      <c r="M271" s="7"/>
+    </row>
+    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B272" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="C272" s="76"/>
+      <c r="D272" s="76"/>
+      <c r="E272" s="76"/>
+      <c r="F272" s="76"/>
+      <c r="G272" s="76"/>
+      <c r="H272" s="76"/>
+      <c r="I272" s="76"/>
+      <c r="J272" s="76"/>
+      <c r="K272" s="76"/>
+      <c r="L272" s="76"/>
+      <c r="M272" s="76"/>
+    </row>
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B273" s="8"/>
+      <c r="C273" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E273" s="4"/>
+      <c r="F273" s="9"/>
+      <c r="G273" s="10"/>
+      <c r="H273" s="10"/>
+      <c r="I273" s="10"/>
+      <c r="J273" s="10"/>
+      <c r="K273" s="10"/>
+      <c r="L273" s="10"/>
+      <c r="M273" s="11"/>
+    </row>
+    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B274" s="13"/>
+      <c r="C274" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D274" s="12"/>
+      <c r="E274" s="15"/>
+      <c r="F274" s="16"/>
+      <c r="G274" s="17"/>
+      <c r="H274" s="17"/>
+      <c r="I274" s="17"/>
+      <c r="J274" s="17"/>
+      <c r="K274" s="17"/>
+      <c r="L274" s="17"/>
+      <c r="M274" s="18"/>
+    </row>
+    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B275" s="13"/>
+      <c r="C275" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D275" s="12"/>
+      <c r="E275" s="15"/>
+      <c r="F275" s="19"/>
+      <c r="G275" s="6"/>
+      <c r="H275" s="6"/>
+      <c r="I275" s="6"/>
+      <c r="J275" s="6"/>
+      <c r="K275" s="6"/>
+      <c r="L275" s="6"/>
+      <c r="M275" s="7"/>
+    </row>
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B276" s="13"/>
+      <c r="C276" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D276" s="12"/>
+      <c r="E276" s="15"/>
+      <c r="F276" s="19"/>
+      <c r="G276" s="6"/>
+      <c r="H276" s="6"/>
+      <c r="I276" s="6"/>
+      <c r="J276" s="6"/>
+      <c r="K276" s="6"/>
+      <c r="L276" s="6"/>
+      <c r="M276" s="7"/>
+    </row>
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="B277" s="13"/>
+      <c r="C277" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D277" s="75"/>
+      <c r="E277" s="15"/>
+      <c r="F277" s="19"/>
+      <c r="G277" s="6"/>
+      <c r="H277" s="6"/>
+      <c r="I277" s="6"/>
+      <c r="J277" s="6"/>
+      <c r="K277" s="6"/>
+      <c r="L277" s="6"/>
+      <c r="M277" s="7"/>
+    </row>
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B278" s="2"/>
+      <c r="C278" s="2"/>
+      <c r="D278" s="2"/>
+      <c r="E278" s="2"/>
+      <c r="F278" s="2"/>
+      <c r="G278" s="2"/>
+      <c r="H278" s="2"/>
+      <c r="I278" s="2"/>
+      <c r="J278" s="2"/>
+      <c r="K278" s="2"/>
+      <c r="L278" s="2"/>
+      <c r="M278" s="2"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="114">
+  <mergeCells count="124">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:H3"/>
@@ -6327,12 +6620,23 @@
     <mergeCell ref="A256:B256"/>
     <mergeCell ref="D256:E256"/>
     <mergeCell ref="A264:M264"/>
+    <mergeCell ref="B268:M268"/>
+    <mergeCell ref="B269:M269"/>
+    <mergeCell ref="B270:H270"/>
+    <mergeCell ref="J270:M270"/>
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="E271:F271"/>
+    <mergeCell ref="B272:M272"/>
+    <mergeCell ref="A273:B273"/>
+    <mergeCell ref="D273:E273"/>
+    <mergeCell ref="A278:M278"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A19" r:id="rId1" display="4 Northern Ireland reformed its local government boundaries in April 2015. Estimates have been provided by the 11 newly created boundaries. For more information see http://www.doeni.gov.uk/local_government_reform"/>
     <hyperlink ref="B30" r:id="rId2" display="http://www.bbc.co.uk/news/uk-41203240"/>
     <hyperlink ref="B93" r:id="rId3" display="https://www.getthedata.com/open-pubs"/>
     <hyperlink ref="B108" r:id="rId4" display="https://data.gov.uk/dataset/hospitals_"/>
+    <hyperlink ref="B272" r:id="rId5" display="https://www.timeshighereducation.com/student/best-universities/best-universities-uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>